<commit_message>
Updated Final Paper for submission
</commit_message>
<xml_diff>
--- a/results/BL_BS_B5_553_results.xlsx
+++ b/results/BL_BS_B5_553_results.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/437b0d8cdafbd5b9/Documents/Personal/Learning/UC Berkeley/MIDS/Courses/W266/Final Project/results/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sundeepm\source\MIDS\w266\w266-final-project\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="30" documentId="11_72F6F92553B1D48D4A047CE5A9D9FA74264E059D" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{683636D7-6242-49C6-A18E-FEBEDC8EC528}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5FFA77E-8DBD-4369-9235-9C75DC9A23D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3340" yWindow="3340" windowWidth="16920" windowHeight="10540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -7561,7 +7561,7 @@
       <name val="Calibri"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -7571,6 +7571,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -7602,7 +7608,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -7611,6 +7617,10 @@
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -7916,13 +7926,14 @@
   <dimension ref="A1:U554"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K1" sqref="K1:K1048576"/>
+      <pane ySplit="1" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I1" sqref="I1:I1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="8" max="8" width="19.6328125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="21.26953125" customWidth="1"/>
     <col min="11" max="11" width="17.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -7948,7 +7959,7 @@
       <c r="H1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="4" t="s">
         <v>7</v>
       </c>
       <c r="J1" s="1" t="s">
@@ -8009,9 +8020,7 @@
         <v>-100</v>
       </c>
       <c r="H2" s="3"/>
-      <c r="I2">
-        <v>-100</v>
-      </c>
+      <c r="I2" s="5"/>
       <c r="J2">
         <v>-100</v>
       </c>
@@ -8065,9 +8074,7 @@
         <v>-100</v>
       </c>
       <c r="H3" s="3"/>
-      <c r="I3">
-        <v>-100</v>
-      </c>
+      <c r="I3" s="5"/>
       <c r="J3">
         <v>-100</v>
       </c>
@@ -8121,9 +8128,7 @@
         <v>-100</v>
       </c>
       <c r="H4" s="3"/>
-      <c r="I4">
-        <v>-100</v>
-      </c>
+      <c r="I4" s="5"/>
       <c r="J4">
         <v>-100</v>
       </c>
@@ -8177,9 +8182,7 @@
         <v>-100</v>
       </c>
       <c r="H5" s="3"/>
-      <c r="I5">
-        <v>-100</v>
-      </c>
+      <c r="I5" s="5"/>
       <c r="J5">
         <v>-100</v>
       </c>
@@ -8233,9 +8236,7 @@
         <v>-100</v>
       </c>
       <c r="H6" s="3"/>
-      <c r="I6">
-        <v>-100</v>
-      </c>
+      <c r="I6" s="5"/>
       <c r="J6">
         <v>-100</v>
       </c>
@@ -8289,9 +8290,7 @@
         <v>-100</v>
       </c>
       <c r="H7" s="3"/>
-      <c r="I7">
-        <v>-100</v>
-      </c>
+      <c r="I7" s="5"/>
       <c r="J7">
         <v>-100</v>
       </c>
@@ -8345,9 +8344,7 @@
         <v>-100</v>
       </c>
       <c r="H8" s="3"/>
-      <c r="I8">
-        <v>-100</v>
-      </c>
+      <c r="I8" s="5"/>
       <c r="J8">
         <v>-100</v>
       </c>
@@ -8401,9 +8398,7 @@
         <v>-100</v>
       </c>
       <c r="H9" s="3"/>
-      <c r="I9">
-        <v>-100</v>
-      </c>
+      <c r="I9" s="5"/>
       <c r="J9">
         <v>-100</v>
       </c>
@@ -8457,9 +8452,7 @@
         <v>-100</v>
       </c>
       <c r="H10" s="3"/>
-      <c r="I10">
-        <v>-100</v>
-      </c>
+      <c r="I10" s="5"/>
       <c r="J10">
         <v>-100</v>
       </c>
@@ -8513,9 +8506,7 @@
         <v>-100</v>
       </c>
       <c r="H11" s="3"/>
-      <c r="I11">
-        <v>-100</v>
-      </c>
+      <c r="I11" s="5"/>
       <c r="J11">
         <v>-100</v>
       </c>
@@ -8569,9 +8560,7 @@
         <v>-100</v>
       </c>
       <c r="H12" s="3"/>
-      <c r="I12">
-        <v>-100</v>
-      </c>
+      <c r="I12" s="5"/>
       <c r="J12">
         <v>-100</v>
       </c>
@@ -8625,9 +8614,7 @@
         <v>-100</v>
       </c>
       <c r="H13" s="3"/>
-      <c r="I13">
-        <v>-100</v>
-      </c>
+      <c r="I13" s="5"/>
       <c r="J13">
         <v>-100</v>
       </c>
@@ -8681,9 +8668,7 @@
         <v>-100</v>
       </c>
       <c r="H14" s="3"/>
-      <c r="I14">
-        <v>-100</v>
-      </c>
+      <c r="I14" s="5"/>
       <c r="J14">
         <v>-100</v>
       </c>
@@ -8737,9 +8722,7 @@
         <v>-100</v>
       </c>
       <c r="H15" s="3"/>
-      <c r="I15">
-        <v>-100</v>
-      </c>
+      <c r="I15" s="5"/>
       <c r="J15">
         <v>-100</v>
       </c>
@@ -8793,9 +8776,7 @@
         <v>-100</v>
       </c>
       <c r="H16" s="3"/>
-      <c r="I16">
-        <v>-100</v>
-      </c>
+      <c r="I16" s="5"/>
       <c r="J16">
         <v>-100</v>
       </c>
@@ -8849,9 +8830,7 @@
         <v>-100</v>
       </c>
       <c r="H17" s="3"/>
-      <c r="I17">
-        <v>-100</v>
-      </c>
+      <c r="I17" s="5"/>
       <c r="J17">
         <v>-100</v>
       </c>
@@ -8905,9 +8884,7 @@
         <v>-100</v>
       </c>
       <c r="H18" s="3"/>
-      <c r="I18">
-        <v>-100</v>
-      </c>
+      <c r="I18" s="5"/>
       <c r="J18">
         <v>-100</v>
       </c>
@@ -8961,9 +8938,7 @@
         <v>-100</v>
       </c>
       <c r="H19" s="3"/>
-      <c r="I19">
-        <v>-100</v>
-      </c>
+      <c r="I19" s="5"/>
       <c r="J19">
         <v>-100</v>
       </c>
@@ -9017,9 +8992,7 @@
         <v>-100</v>
       </c>
       <c r="H20" s="3"/>
-      <c r="I20">
-        <v>-100</v>
-      </c>
+      <c r="I20" s="5"/>
       <c r="J20">
         <v>-100</v>
       </c>
@@ -9073,9 +9046,7 @@
         <v>-100</v>
       </c>
       <c r="H21" s="3"/>
-      <c r="I21">
-        <v>-100</v>
-      </c>
+      <c r="I21" s="5"/>
       <c r="J21">
         <v>-100</v>
       </c>
@@ -9129,9 +9100,7 @@
         <v>-100</v>
       </c>
       <c r="H22" s="3"/>
-      <c r="I22">
-        <v>-100</v>
-      </c>
+      <c r="I22" s="5"/>
       <c r="J22">
         <v>-100</v>
       </c>
@@ -9185,9 +9154,7 @@
         <v>-100</v>
       </c>
       <c r="H23" s="3"/>
-      <c r="I23">
-        <v>-100</v>
-      </c>
+      <c r="I23" s="5"/>
       <c r="J23">
         <v>-100</v>
       </c>
@@ -9241,9 +9208,7 @@
         <v>-100</v>
       </c>
       <c r="H24" s="3"/>
-      <c r="I24">
-        <v>-100</v>
-      </c>
+      <c r="I24" s="5"/>
       <c r="J24">
         <v>-100</v>
       </c>

</xml_diff>